<commit_message>
updates in documentation etc.
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Amount of Iterations</t>
   </si>
@@ -56,7 +56,10 @@
     <t>folder name</t>
   </si>
   <si>
-    <t>21_01-223435</t>
+    <t>4 i7 CPUs, 16 GRAM</t>
+  </si>
+  <si>
+    <t>results_22_01-205446</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,10 +391,10 @@
     <col min="5" max="5" width="21.453125" customWidth="1"/>
     <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.1796875" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -417,7 +420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -425,22 +428,25 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>29.79</v>
       </c>
       <c r="D2" s="1">
-        <v>0.75416666666666676</v>
+        <v>0.85486111111111107</v>
       </c>
       <c r="E2" s="1">
-        <v>6.2499999999999995E-3</v>
+        <v>0.25416666666666665</v>
       </c>
       <c r="F2" s="1">
-        <v>4.8611111111111112E-3</v>
+        <v>0.19930555555555554</v>
       </c>
       <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature attempts to fix "," mistakes
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="7410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14730" windowHeight="7410" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="POSSIBLY NON RELEVANT FEATURES" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t>Model</t>
   </si>
@@ -249,6 +250,15 @@
   </si>
   <si>
     <t>results_25_01-004202</t>
+  </si>
+  <si>
+    <t>פיצ'רים שהיו בשימוש</t>
+  </si>
+  <si>
+    <t>1, 4, 7, 8, 10, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43</t>
+  </si>
+  <si>
+    <t>14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 31, 32, 33, 34, 35, 40, 41, 42, 43</t>
   </si>
 </sst>
 </file>
@@ -284,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +306,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,4 +1451,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Results + Report update
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="125">
   <si>
     <t>Model</t>
   </si>
@@ -385,6 +385,21 @@
   </si>
   <si>
     <t>results_27_01-090843</t>
+  </si>
+  <si>
+    <t>1-26,28-32,40-53</t>
+  </si>
+  <si>
+    <t>80.1</t>
+  </si>
+  <si>
+    <t>1:49:33</t>
+  </si>
+  <si>
+    <t>1:16</t>
+  </si>
+  <si>
+    <t>results_27_01-154450</t>
   </si>
 </sst>
 </file>
@@ -718,7 +733,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1685,17 +1700,39 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="A34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>

</xml_diff>

<commit_message>
minor fixes so that pycharm will be happy ;)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="143">
   <si>
     <t>Model</t>
   </si>
@@ -435,9 +435,6 @@
     <t>80.56</t>
   </si>
   <si>
-    <t>1-26, 28-36, 41-53</t>
-  </si>
-  <si>
     <t>1:29:24</t>
   </si>
   <si>
@@ -448,6 +445,15 @@
   </si>
   <si>
     <t>results_28_01-090418</t>
+  </si>
+  <si>
+    <t>27 - not good</t>
+  </si>
+  <si>
+    <t>40 - irrelevnat</t>
+  </si>
+  <si>
+    <t>1-26, 28-36, 41-48, 50-53</t>
   </si>
 </sst>
 </file>
@@ -780,14 +786,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H22" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" customWidth="1"/>
     <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" customWidth="1"/>
     <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
@@ -1800,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>80</v>
@@ -1835,7 +1841,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>80</v>
@@ -1850,19 +1856,19 @@
         <v>135</v>
       </c>
       <c r="G37" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -1921,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1934,7 +1940,7 @@
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1945,47 +1951,53 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>27</v>
       </c>

</xml_diff>